<commit_message>
added new figures for the sponge and fish predictions that split up the sites to make it easier to see CI's; made models in AIC tables more interpretable
</commit_message>
<xml_diff>
--- a/Results_May_15_mostrecentupdateMay22/combined_all.xlsx
+++ b/Results_May_15_mostrecentupdateMay22/combined_all.xlsx
@@ -40,70 +40,70 @@
     <t>Cum.Wt</t>
   </si>
   <si>
-    <t>cc_yr_site</t>
-  </si>
-  <si>
-    <t>r_yr_site</t>
-  </si>
-  <si>
-    <t>cc_site</t>
-  </si>
-  <si>
-    <t>yr_site</t>
-  </si>
-  <si>
-    <t>sc_yr_site</t>
-  </si>
-  <si>
-    <t>yr_site_yrxsite</t>
-  </si>
-  <si>
     <t>site</t>
   </si>
   <si>
-    <t>sc_site</t>
-  </si>
-  <si>
-    <t>r_site</t>
-  </si>
-  <si>
-    <t>r_yr</t>
-  </si>
-  <si>
-    <t>r_site_sitexr</t>
-  </si>
-  <si>
-    <t>cc_site_sitexcc</t>
-  </si>
-  <si>
-    <t>r_yr_yrxr</t>
-  </si>
-  <si>
-    <t>sc_site_sitexsc</t>
-  </si>
-  <si>
-    <t>cc_yr</t>
-  </si>
-  <si>
-    <t>cc_yr_yrxcc</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>yr</t>
-  </si>
-  <si>
-    <t>sc_yr</t>
-  </si>
-  <si>
-    <t>sc_yr_yrxsc</t>
-  </si>
-  <si>
-    <t>sc</t>
+    <t>year + site</t>
+  </si>
+  <si>
+    <t>year + site + year*site</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>coralcover + year + site</t>
+  </si>
+  <si>
+    <t>coralcover + site</t>
+  </si>
+  <si>
+    <t>coralcover + site + site*coralcover</t>
+  </si>
+  <si>
+    <t>coralcover + year</t>
+  </si>
+  <si>
+    <t>coralcover + year + year*coralcover</t>
+  </si>
+  <si>
+    <t>coralcover</t>
+  </si>
+  <si>
+    <t>spongecover + year + site</t>
+  </si>
+  <si>
+    <t>spongecover + site</t>
+  </si>
+  <si>
+    <t>spongecover + site + site*spongecover</t>
+  </si>
+  <si>
+    <t>spongecover + year</t>
+  </si>
+  <si>
+    <t>spongecover + year + year*spongecover</t>
+  </si>
+  <si>
+    <t>spongecover</t>
+  </si>
+  <si>
+    <t>rugosity + year + site</t>
+  </si>
+  <si>
+    <t>rugosity + site</t>
+  </si>
+  <si>
+    <t>rugosity + year</t>
+  </si>
+  <si>
+    <t>rugosity + site + site*rugosity</t>
+  </si>
+  <si>
+    <t>rugosity + year + year*rugosity</t>
+  </si>
+  <si>
+    <t>rugosity</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -634,9 +634,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -985,7 +985,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>11</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>11</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>10</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>11</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>17</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>9</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2">
         <v>17</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>17</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <v>17</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>5</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2">
         <v>3</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
         <v>4</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2">
         <v>5</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>

</xml_diff>